<commit_message>
Correções nos modelos de importação para adequação ao formato do inep.
</commit_message>
<xml_diff>
--- a/modelos/docentes_pos_graduacao.xlsx
+++ b/modelos/docentes_pos_graduacao.xlsx
@@ -35,11 +35,6 @@
 Ex: 01/01/2017</t>
   </si>
   <si>
-    <t>0 ­ Especialização
-1 ­ Mestrado
-2 ­ Doutorado</t>
-  </si>
-  <si>
     <t>Codigo de matrícula do docente na UEFS</t>
   </si>
   <si>
@@ -53,6 +48,11 @@
   </si>
   <si>
     <t>De onde vieram essas informações?</t>
+  </si>
+  <si>
+    <t>1 ­ Especialização
+2 ­ Mestrado
+3 ­ Doutorado</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -496,7 +496,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="21.75" customHeight="1">
@@ -510,24 +510,24 @@
     </row>
     <row r="3" spans="1:5" ht="38.25">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="26.25" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>

</xml_diff>